<commit_message>
Rewrote transmission code (now in TxWorking). GPS and LoRa stuff working. Rx End developed.
</commit_message>
<xml_diff>
--- a/software/Packet Schema.xlsx
+++ b/software/Packet Schema.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Byte id</t>
   </si>
@@ -34,13 +34,37 @@
   </si>
   <si>
     <t xml:space="preserve">Pressure </t>
+  </si>
+  <si>
+    <t>Len (bits)</t>
+  </si>
+  <si>
+    <t>GPS lat</t>
+  </si>
+  <si>
+    <t>degrees * 1e6</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>dPa (Pa / 10)</t>
+  </si>
+  <si>
+    <t>GPS Lng</t>
+  </si>
+  <si>
+    <t>All data big-endian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -52,6 +76,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,14 +114,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -411,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -423,7 +471,7 @@
     <col min="2" max="2" width="67.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,9 +481,14 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -445,8 +498,17 @@
       <c r="C2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -457,7 +519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
@@ -468,7 +530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>3</v>
       </c>
@@ -479,7 +541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>4</v>
       </c>
@@ -489,8 +551,14 @@
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>5</v>
       </c>
@@ -501,47 +569,89 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>14</v>
       </c>
@@ -628,6 +738,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>